<commit_message>
Enhance transaction management features and improve configuration handling (CSV Only)
</commit_message>
<xml_diff>
--- a/storage/data/saku_data.xlsx
+++ b/storage/data/saku_data.xlsx
@@ -474,7 +474,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45444</v>
+        <v>45324</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -483,15 +483,15 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>food</t>
+          <t>groceries</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>15000</v>
+        <v>150</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Lunch at cafe</t>
+          <t>February groceries note</t>
         </is>
       </c>
     </row>

</xml_diff>